<commit_message>
Dimension 4 fixed, FULLY COMPLETE
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb9da5768798d098/Harvard/Sophmore/Spring/A. CS124/CS124-P1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="8_{1BA6EBC2-B54E-44F0-9434-8F2A8AA229B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{738D6F3B-1D4E-4B4E-9D4C-19397A874DA3}"/>
+  <xr:revisionPtr revIDLastSave="344" documentId="8_{1BA6EBC2-B54E-44F0-9434-8F2A8AA229B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7760E72E-9DBD-4F7D-9E80-03FA0DCCEE1D}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{09920646-C4B9-4870-B214-B70F80188ABD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{09920646-C4B9-4870-B214-B70F80188ABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Dim 1" sheetId="2" r:id="rId1"/>
@@ -70,6 +70,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,16 +126,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -238,28 +244,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C58A119A-EF1A-42CC-BAFE-28A5519322EB}" name="Table13" displayName="Table13" ref="B3:F63" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C58A119A-EF1A-42CC-BAFE-28A5519322EB}" name="Table13" displayName="Table13" ref="B3:F63" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="B3:F63" xr:uid="{C58A119A-EF1A-42CC-BAFE-28A5519322EB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5ED73DD7-DE97-4158-B35C-94DF9A1103D6}" name="Num points" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{91476B41-D7EF-4225-9799-A62D26AD0DA7}" name="Dimension" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{12A188E7-49BB-4E44-8443-C5889BA396E8}" name="Output" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{5DE9B7A1-2663-4B42-B25E-E709B369F36A}" name="Trial number" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{C23680BA-21F2-4448-814F-664A761857D2}" name="Time" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{5ED73DD7-DE97-4158-B35C-94DF9A1103D6}" name="Num points" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{91476B41-D7EF-4225-9799-A62D26AD0DA7}" name="Dimension" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{12A188E7-49BB-4E44-8443-C5889BA396E8}" name="Output" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{5DE9B7A1-2663-4B42-B25E-E709B369F36A}" name="Trial number" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{C23680BA-21F2-4448-814F-664A761857D2}" name="Time" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E91F08EB-15BF-4495-AA54-634F8FF12B78}" name="Table1" displayName="Table1" ref="B2:F63" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E91F08EB-15BF-4495-AA54-634F8FF12B78}" name="Table1" displayName="Table1" ref="B2:F63" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B2:F63" xr:uid="{E91F08EB-15BF-4495-AA54-634F8FF12B78}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B90BE400-1EF3-4B58-B374-FCC85E6A2C50}" name="Num points" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{C6BD413B-97D7-4AF5-915C-3B5E4F50C27B}" name="Dimension" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{D19086EE-B153-40CA-8DAE-6AD79AC34F60}" name="Output" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{A71962CE-E240-485F-817C-28A9B5E758A2}" name="Trial number" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{13634A39-BD4A-417B-8A65-EFCCC1B4C8DD}" name="Time" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{B90BE400-1EF3-4B58-B374-FCC85E6A2C50}" name="Num points" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C6BD413B-97D7-4AF5-915C-3B5E4F50C27B}" name="Dimension" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{D19086EE-B153-40CA-8DAE-6AD79AC34F60}" name="Output" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A71962CE-E240-485F-817C-28A9B5E758A2}" name="Trial number" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{13634A39-BD4A-417B-8A65-EFCCC1B4C8DD}" name="Time" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -592,655 +598,682 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1BDCA0-94AB-4AE3-8011-063984309417}">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="17.44140625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="17.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>128</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.979186</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>128</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.98504599999999998</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>128</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.99526999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>128</v>
       </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
         <v>0.97353999999999996</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>128</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
         <v>0.994232</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>256</v>
       </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.99056999999999995</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>256</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.98706000000000005</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>256</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
         <v>0.99862700000000004</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>256</v>
       </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
         <v>0.99862700000000004</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>256</v>
       </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
         <v>0.991699</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>512</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
         <v>0.99633799999999995</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>512</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
         <v>0.98730399999999996</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>512</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
         <v>0.99795500000000004</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>512</v>
       </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
         <v>0.99795500000000004</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>512</v>
       </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
         <v>0.99688600000000005</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1024</v>
       </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
         <v>0.99874799999999997</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1024</v>
       </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
         <v>0.99886799999999998</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1024</v>
       </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
         <v>0.99938700000000003</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1024</v>
       </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
         <v>0.99935700000000005</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>1024</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
         <v>0.99938700000000003</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>2048</v>
       </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
         <v>0.99898799999999999</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>2048</v>
       </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
         <v>0.99917199999999995</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2048</v>
       </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
         <v>0.99929500000000004</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>2048</v>
       </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
         <v>0.99926099999999995</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>2048</v>
       </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
         <v>0.99938499999999997</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>4096</v>
       </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
         <v>0.99950600000000001</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>4096</v>
       </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
         <v>0.99870599999999998</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4096</v>
       </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
         <v>0.99983599999999995</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>4096</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
         <v>0.99983599999999995</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>4096</v>
       </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
         <v>0.99986399999999998</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>8192</v>
       </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
         <v>0.99989600000000001</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>8192</v>
       </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2">
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
         <v>0.99992599999999998</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>8192</v>
       </c>
-      <c r="C36" s="2">
-        <v>1</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
         <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>8192</v>
       </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2">
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
         <v>0.99980899999999995</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>8192</v>
       </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
-      <c r="D38" s="2">
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
         <v>0.99980199999999997</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>16384</v>
       </c>
-      <c r="C39" s="2">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
         <v>0.99968599999999996</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>16384</v>
       </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2">
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
         <v>0.99995400000000001</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>16384</v>
       </c>
-      <c r="C41" s="2">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
         <v>0.99986299999999995</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>16384</v>
       </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
         <v>0.99995599999999996</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>16384</v>
       </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2">
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
         <v>0.99992499999999995</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>32768</v>
       </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2">
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
         <v>0.99996200000000002</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>32768</v>
       </c>
-      <c r="C45" s="2">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2">
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
         <v>0.99999199999999999</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>32768</v>
       </c>
-      <c r="C46" s="2">
-        <v>1</v>
-      </c>
-      <c r="D46" s="2">
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
         <v>0.99995599999999996</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>32768</v>
       </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2">
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
         <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>32768</v>
       </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2">
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
         <v>0.99992800000000004</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>65536</v>
       </c>
-      <c r="C49" s="2">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2">
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
         <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>65536</v>
       </c>
-      <c r="C50" s="2">
-        <v>1</v>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.99995999999999996</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>65536</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>65536</v>
       </c>
-      <c r="C52" s="2">
-        <v>1</v>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.99995699999999998</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>65536</v>
       </c>
-      <c r="C53" s="2">
-        <v>1</v>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.99995599999999996</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>131072</v>
       </c>
-      <c r="C54" s="2">
-        <v>1</v>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>131072</v>
       </c>
-      <c r="C55" s="2">
-        <v>1</v>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>131072</v>
       </c>
-      <c r="C56" s="2">
-        <v>1</v>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.99998500000000001</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>131072</v>
       </c>
-      <c r="C57" s="2">
-        <v>1</v>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.999996</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>131072</v>
       </c>
-      <c r="C58" s="2">
-        <v>1</v>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.999996</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>262144</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>262144</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>262144</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>262144</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>262144</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1260,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95B58CA-6085-4D62-A028-1C980CFC9E5E}">
   <dimension ref="B1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
@@ -1271,771 +1304,787 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>128</v>
       </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
         <v>7.5890110000000002</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>128</v>
       </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
         <v>7.5187220000000003</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>128</v>
       </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
         <v>7.5598510000000001</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>128</v>
       </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <v>7.6154919999999997</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>128</v>
       </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
         <v>7.2969460000000002</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>256</v>
       </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
         <v>11.077892</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>256</v>
       </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
         <v>10.604752</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>256</v>
       </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
         <v>10.561726999999999</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>256</v>
       </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
         <v>10.686709</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>256</v>
       </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
         <v>10.453925999999999</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>512</v>
       </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
         <v>15.356678</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>512</v>
       </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
         <v>14.814192</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>512</v>
       </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
         <v>15.146169</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>512</v>
       </c>
-      <c r="C16" s="2">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
         <v>15.066515000000001</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>512</v>
       </c>
-      <c r="C17" s="2">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
         <v>15.013754</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1024</v>
       </c>
-      <c r="C18" s="2">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
         <v>20.961193000000002</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1024</v>
       </c>
-      <c r="C19" s="2">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
         <v>21.195736</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1024</v>
       </c>
-      <c r="C20" s="2">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
         <v>20.938569999999999</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1024</v>
       </c>
-      <c r="C21" s="2">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
         <v>21.426438999999998</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1024</v>
       </c>
-      <c r="C22" s="2">
-        <v>2</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
         <v>20.861350999999999</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>2048</v>
       </c>
-      <c r="C23" s="2">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
         <v>29.565764999999999</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>2048</v>
       </c>
-      <c r="C24" s="2">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
         <v>29.761210999999999</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>2048</v>
       </c>
-      <c r="C25" s="2">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
         <v>29.627016000000001</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2048</v>
       </c>
-      <c r="C26" s="2">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
         <v>29.484895999999999</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>2048</v>
       </c>
-      <c r="C27" s="2">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
         <v>29.536638</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>4096</v>
       </c>
-      <c r="C28" s="2">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
         <v>41.787757999999997</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>4096</v>
       </c>
-      <c r="C29" s="2">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
         <v>41.930045999999997</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>4096</v>
       </c>
-      <c r="C30" s="2">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
         <v>41.578014000000003</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4096</v>
       </c>
-      <c r="C31" s="2">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
         <v>41.833663999999999</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>4096</v>
       </c>
-      <c r="C32" s="2">
-        <v>2</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
         <v>42.094326000000002</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>8192</v>
       </c>
-      <c r="C33" s="2">
-        <v>2</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>58.852291000000001</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>8192</v>
       </c>
-      <c r="C34" s="2">
-        <v>2</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>58.997501</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>8192</v>
       </c>
-      <c r="C35" s="2">
-        <v>2</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>58.646056999999999</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>8192</v>
       </c>
-      <c r="C36" s="2">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>58.642001999999998</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>8192</v>
       </c>
-      <c r="C37" s="2">
-        <v>2</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>58.814109999999999</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>16384</v>
       </c>
-      <c r="C38" s="2">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>83.204689000000002</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>16384</v>
       </c>
-      <c r="C39" s="2">
-        <v>2</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>83.078781000000006</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>16384</v>
       </c>
-      <c r="C40" s="2">
-        <v>2</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>83.339095999999998</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>16384</v>
       </c>
-      <c r="C41" s="2">
-        <v>2</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
         <v>83.198166000000001</v>
       </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2"/>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>16384</v>
       </c>
-      <c r="C42" s="2">
-        <v>2</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>32768</v>
       </c>
-      <c r="C43" s="2">
-        <v>2</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>32768</v>
       </c>
-      <c r="C44" s="2">
-        <v>2</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>32768</v>
       </c>
-      <c r="C45" s="2">
-        <v>2</v>
-      </c>
-      <c r="D45" s="2">
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1">
         <v>117.33820299999999</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>32768</v>
       </c>
-      <c r="C46" s="2">
-        <v>2</v>
-      </c>
-      <c r="D46" s="2">
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
         <v>117.42409499999999</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>32768</v>
       </c>
-      <c r="C47" s="2">
-        <v>2</v>
-      </c>
-      <c r="D47" s="2">
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
         <v>117.304306</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>65536</v>
       </c>
-      <c r="C48" s="2">
-        <v>2</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>65536</v>
       </c>
-      <c r="C49" s="2">
-        <v>2</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>65536</v>
       </c>
-      <c r="C50" s="2">
-        <v>2</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="C50" s="1">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>65536</v>
       </c>
-      <c r="C51" s="2">
-        <v>2</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>65536</v>
       </c>
-      <c r="C52" s="2">
-        <v>2</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>131072</v>
       </c>
-      <c r="C53" s="2">
-        <v>2</v>
-      </c>
-      <c r="D53" s="2">
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
         <v>234.77619899999999</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>131072</v>
       </c>
-      <c r="C54" s="2">
-        <v>2</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="C54" s="1">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>131072</v>
       </c>
-      <c r="C55" s="2">
-        <v>2</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>131072</v>
       </c>
-      <c r="C56" s="2">
-        <v>2</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="C56" s="1">
+        <v>2</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>131072</v>
       </c>
-      <c r="C57" s="2">
-        <v>2</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="C57" s="1">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>262144</v>
       </c>
-      <c r="C58" s="2">
-        <v>2</v>
-      </c>
-      <c r="D58" s="2">
+      <c r="C58" s="1">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1">
         <v>331.14349399999998</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>262144</v>
       </c>
-      <c r="C59" s="2">
-        <v>2</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>262144</v>
       </c>
-      <c r="C60" s="2">
-        <v>2</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="C60" s="1">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>262144</v>
       </c>
-      <c r="C61" s="2">
-        <v>2</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="C61" s="1">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>262144</v>
       </c>
-      <c r="C62" s="2">
-        <v>2</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="C62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2053,658 +2102,658 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE35272-887C-4BCA-9730-4FEC6E41DD03}">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="17.44140625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="17.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>128</v>
       </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
         <v>18.249410999999998</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>128</v>
       </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
         <v>18.061060000000001</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>128</v>
       </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
         <v>17.140604</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>128</v>
       </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
         <v>17.713892000000001</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>128</v>
       </c>
-      <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>17.841464999999999</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>256</v>
       </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
         <v>27.970533</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>256</v>
       </c>
-      <c r="C10" s="2">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
         <v>28.202369999999998</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>256</v>
       </c>
-      <c r="C11" s="2">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
         <v>27.233270999999998</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>256</v>
       </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
         <v>28.113195000000001</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>256</v>
       </c>
-      <c r="C13" s="2">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
         <v>27.971862999999999</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>512</v>
       </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
         <v>43.644984999999998</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>512</v>
       </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
         <v>43.334702</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>512</v>
       </c>
-      <c r="C16" s="2">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
         <v>44.300865000000002</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>512</v>
       </c>
-      <c r="C17" s="2">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
         <v>43.390090999999998</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>512</v>
       </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
         <v>43.929478000000003</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1024</v>
       </c>
-      <c r="C19" s="2">
-        <v>3</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
         <v>68.186286999999993</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1024</v>
       </c>
-      <c r="C20" s="2">
-        <v>3</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
         <v>68.574462999999994</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1024</v>
       </c>
-      <c r="C21" s="2">
-        <v>3</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
         <v>68.426040999999998</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1024</v>
       </c>
-      <c r="C22" s="2">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
         <v>68.279114000000007</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>1024</v>
       </c>
-      <c r="C23" s="2">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
         <v>68.582381999999996</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>2048</v>
       </c>
-      <c r="C24" s="2">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
         <v>106.893394</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>2048</v>
       </c>
-      <c r="C25" s="2">
-        <v>3</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
         <v>108.016289</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2048</v>
       </c>
-      <c r="C26" s="2">
-        <v>3</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1">
         <v>107.58203899999999</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>2048</v>
       </c>
-      <c r="C27" s="2">
-        <v>3</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
         <v>107.381989</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>2048</v>
       </c>
-      <c r="C28" s="2">
-        <v>3</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
         <v>107.161209</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>4096</v>
       </c>
-      <c r="C29" s="2">
-        <v>3</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
         <v>168.275116</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>4096</v>
       </c>
-      <c r="C30" s="2">
-        <v>3</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
         <v>168.54754600000001</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4096</v>
       </c>
-      <c r="C31" s="2">
-        <v>3</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1">
         <v>168.43019100000001</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>4096</v>
       </c>
-      <c r="C32" s="2">
-        <v>3</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
         <v>168.706436</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>4096</v>
       </c>
-      <c r="C33" s="2">
-        <v>3</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
         <v>169.47470100000001</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>8192</v>
       </c>
-      <c r="C34" s="2">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
         <v>267.12481700000001</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>8192</v>
       </c>
-      <c r="C35" s="2">
-        <v>3</v>
-      </c>
-      <c r="D35" s="2">
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
         <v>268.20358299999998</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>8192</v>
       </c>
-      <c r="C36" s="2">
-        <v>3</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1">
         <v>267.76400799999999</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>8192</v>
       </c>
-      <c r="C37" s="2">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2">
+      <c r="C37" s="1">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1">
         <v>268.29244999999997</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>8192</v>
       </c>
-      <c r="C38" s="2">
-        <v>3</v>
-      </c>
-      <c r="D38" s="2">
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
         <v>267.67666600000001</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>16384</v>
       </c>
-      <c r="C39" s="2">
-        <v>3</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1">
         <v>422.48126200000002</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>16384</v>
       </c>
-      <c r="C40" s="2">
-        <v>3</v>
-      </c>
-      <c r="D40" s="2">
+      <c r="C40" s="1">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1">
         <v>423.23507699999999</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>16384</v>
       </c>
-      <c r="C41" s="2">
-        <v>3</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="C41" s="1">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1">
         <v>421.99588</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>16384</v>
       </c>
-      <c r="C42" s="2">
-        <v>3</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="C42" s="1">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1">
         <v>422.049103</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>16384</v>
       </c>
-      <c r="C43" s="2">
-        <v>3</v>
-      </c>
-      <c r="D43" s="2">
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
         <v>421.62243699999999</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>32768</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>32768</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>32768</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>32768</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>32768</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>65536</v>
       </c>
-      <c r="C49" s="2">
-        <v>3</v>
-      </c>
-      <c r="D49" s="2">
+      <c r="C49" s="1">
+        <v>3</v>
+      </c>
+      <c r="D49" s="1">
         <v>1058.169067</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>65536</v>
       </c>
-      <c r="C50" s="2">
-        <v>3</v>
-      </c>
-      <c r="D50" s="2">
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
         <v>1059.307495</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>65536</v>
       </c>
-      <c r="C51" s="2">
-        <v>3</v>
-      </c>
-      <c r="D51" s="2">
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
         <v>1058.661499</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>65536</v>
       </c>
-      <c r="C52" s="2">
-        <v>3</v>
-      </c>
-      <c r="D52" s="2">
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1">
         <v>1060.0708010000001</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>65536</v>
       </c>
-      <c r="C53" s="2">
-        <v>3</v>
-      </c>
-      <c r="D53" s="2">
+      <c r="C53" s="1">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1">
         <v>1059.9060059999999</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>131072</v>
       </c>
-      <c r="C54" s="2">
-        <v>3</v>
-      </c>
-      <c r="D54" s="2">
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
         <v>1677.4357910000001</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>131072</v>
       </c>
-      <c r="C55" s="2">
-        <v>3</v>
-      </c>
-      <c r="D55" s="2">
+      <c r="C55" s="1">
+        <v>3</v>
+      </c>
+      <c r="D55" s="1">
         <v>1675.3885499999999</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>131072</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>131072</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>131072</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>262144</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>262144</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>262144</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>262144</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>262144</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2723,517 +2772,523 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFD9678-EE97-4F1F-9CCB-F22CFD3A5F42}">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="17.44140625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="17.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>128</v>
       </c>
-      <c r="C4" s="2">
-        <v>4</v>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>29.018553000000001</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>128</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>128</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>128</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>128</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>256</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>256</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>256</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>256</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>256</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>512</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>512</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>512</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>512</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>512</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>1024</v>
       </c>
-      <c r="C19" s="2">
-        <v>4</v>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>129.459</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>1024</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>1024</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>1024</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>1024</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>2048</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>2048</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>2048</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>2048</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>2048</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>4096</v>
       </c>
-      <c r="C29" s="2">
-        <v>4</v>
-      </c>
-      <c r="G29" s="3"/>
+      <c r="C29" s="1">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>4096</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4096</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>4096</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>4096</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>8192</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>8192</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>8192</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>8192</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>8192</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>16384</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>16384</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>16384</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>16384</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>16384</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>32768</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>32768</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>32768</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>32768</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>32768</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>65536</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>65536</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>65536</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>65536</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>65536</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>131072</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>131072</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>131072</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>131072</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>131072</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>262144</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>262144</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>262144</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>262144</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>262144</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trials implemented correctly, dimension 1 fix?
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb9da5768798d098/Harvard/Sophmore/Spring/A. CS124/CS124-P1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="344" documentId="8_{1BA6EBC2-B54E-44F0-9434-8F2A8AA229B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7760E72E-9DBD-4F7D-9E80-03FA0DCCEE1D}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="8_{1BA6EBC2-B54E-44F0-9434-8F2A8AA229B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CA4E256-7B0E-477D-A4DB-46F6981DB3B8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{09920646-C4B9-4870-B214-B70F80188ABD}"/>
   </bookViews>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1BDCA0-94AB-4AE3-8011-063984309417}">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,6 +1243,9 @@
       </c>
       <c r="C59" s="1">
         <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.99999800000000005</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
@@ -1293,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95B58CA-6085-4D62-A028-1C980CFC9E5E}">
   <dimension ref="B1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
@@ -2102,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE35272-887C-4BCA-9730-4FEC6E41DD03}">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2723,6 +2726,9 @@
       </c>
       <c r="C59" s="1">
         <v>3</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2658.3466800000001</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
@@ -2772,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFD9678-EE97-4F1F-9CCB-F22CFD3A5F42}">
   <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3044,7 +3050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>4096</v>
       </c>
@@ -3052,7 +3058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>8192</v>
       </c>
@@ -3060,7 +3066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>8192</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>8192</v>
       </c>
@@ -3076,7 +3082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>8192</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>8192</v>
       </c>
@@ -3092,7 +3098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>16384</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>16384</v>
       </c>
@@ -3108,7 +3114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>16384</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>16384</v>
       </c>
@@ -3124,7 +3130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>16384</v>
       </c>
@@ -3132,31 +3138,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>32768</v>
       </c>
       <c r="C44" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="1">
+        <v>1689.7092290000001</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>32768</v>
       </c>
       <c r="C45" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="1">
+        <v>1689.863159</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>32768</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="1">
+        <v>1691.2054439999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>32768</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>32768</v>
       </c>
@@ -3172,15 +3187,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>65536</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="1">
+        <v>2825.0258789999998</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>65536</v>
       </c>
@@ -3188,7 +3206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>65536</v>
       </c>
@@ -3196,7 +3214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>65536</v>
       </c>
@@ -3204,7 +3222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>65536</v>
       </c>
@@ -3212,15 +3230,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>131072</v>
       </c>
       <c r="C54" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="1">
+        <v>4733.6245120000003</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>131072</v>
       </c>
@@ -3228,7 +3249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>131072</v>
       </c>
@@ -3236,7 +3257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>131072</v>
       </c>
@@ -3244,7 +3265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>131072</v>
       </c>
@@ -3252,15 +3273,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>262144</v>
       </c>
       <c r="C59" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D59" s="1">
+        <v>7966.826172</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>262144</v>
       </c>
@@ -3268,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>262144</v>
       </c>
@@ -3276,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>262144</v>
       </c>
@@ -3284,7 +3308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>262144</v>
       </c>

</xml_diff>